<commit_message>
last commit before changes
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -20,51 +20,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Order Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDFOrder</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Customer</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
+    <t xml:space="preserve">P.O. Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship Via</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
   </si>
   <si>
     <t xml:space="preserve">Pack Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Ship Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maya</t>
   </si>
   <si>
-    <t xml:space="preserve">Carrot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 lb case</t>
+    <t xml:space="preserve">CAR25</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
-    <t xml:space="preserve">Lettuce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 head</t>
+    <t xml:space="preserve">LG10</t>
   </si>
   <si>
     <t xml:space="preserve">Terry</t>
   </si>
   <si>
-    <t xml:space="preserve">Snow Peas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 lb case</t>
+    <t xml:space="preserve">L24</t>
   </si>
 </sst>
 </file>
@@ -80,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,14 +105,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,16 +156,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,6 +186,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -179,80 +254,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>44604</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>44604</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>44605</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>44605</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="E4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="n">
         <v>44663</v>
       </c>
     </row>

</xml_diff>